<commit_message>
Rework examples/tests due to reserver 0/0/0 broadcast address
</commit_message>
<xml_diff>
--- a/docs/Examples/01-SmallExampleWithRoomBook/KNX-planning-example.xlsx
+++ b/docs/Examples/01-SmallExampleWithRoomBook/KNX-planning-example.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Room Book" sheetId="2" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'KNX Group Addresses'!$A$7:$J$277</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'KNX Group Addresses'!$A$7:$J$278</definedName>
     <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">'Room Book'!$A$8:$I$11</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_FilterDatabase_0_0" vbProcedure="false">'Room Book'!$B$8:$I$11</definedName>
   </definedNames>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="63">
   <si>
     <t xml:space="preserve">KNX Group Addresses</t>
   </si>
@@ -62,6 +62,12 @@
   </si>
   <si>
     <t xml:space="preserve">Comment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0/0/0 is a reserved KNX broadcast address. Don’t use.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reserved KNX broadcast address</t>
   </si>
   <si>
     <t xml:space="preserve">Light &amp; Power</t>
@@ -696,6 +702,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -706,10 +716,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -1020,10 +1026,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J277"/>
+  <dimension ref="A1:J278"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J20" activeCellId="0" sqref="J20"/>
+      <selection pane="topLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1096,666 +1102,683 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="9"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9" t="str">
-        <f aca="false">IF(AND(ISNUMBER(A8),ISNUMBER(C8),ISNUMBER(E8),ISTEXT(G8)),A8&amp;"/"&amp;C8&amp;"/"&amp;E8,"")</f>
-        <v/>
-      </c>
-      <c r="I8" s="9" t="str">
-        <f aca="false">IF(AND(ISNUMBER(B8),ISNUMBER(D8),ISNUMBER(F8),ISTEXT(H8)),B8&amp;"/"&amp;D8&amp;"/"&amp;F8,"")</f>
-        <v/>
-      </c>
-      <c r="J8" s="9"/>
+      <c r="A8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B8" s="9"/>
+      <c r="C8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" s="9"/>
+      <c r="H8" s="3" t="str">
+        <f aca="false">IF(AND(ISNUMBER(A8),ISNUMBER(C8),ISNUMBER(E8),ISTEXT(F8),ISTEXT(G8)),A8&amp;"/"&amp;C8&amp;"/"&amp;E8,"")</f>
+        <v/>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F9" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="G9" s="1" t="str">
-        <f aca="false">'Room Book'!$A$9</f>
-        <v>B0-0-L</v>
-      </c>
-      <c r="H9" s="3" t="str">
-        <f aca="false">IF(AND(ISNUMBER(A9),ISNUMBER(C9),ISNUMBER(E9),ISTEXT(F9),ISTEXT(G9)),A9&amp;"/"&amp;C9&amp;"/"&amp;E9,"")</f>
-        <v>0/0/0</v>
-      </c>
-      <c r="I9" s="2" t="str">
-        <f aca="false">IF(ISTEXT(G9),VLOOKUP($G9,'Room Book'!$A$7:$I$634,2,0)&amp;" "&amp;VLOOKUP($G9,'Room Book'!$A$7:$I$634,3,0)&amp;" - "&amp;VLOOKUP($G9,'Room Book'!$A$7:$I655,8,0)&amp;" - "&amp;B9&amp;" "&amp;D9,{})</f>
-        <v>Basement Office - Ceiling light - Light &amp; Power Switch</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>15</v>
-      </c>
+      <c r="A9" s="10"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B10" s="12" t="s">
-        <v>12</v>
+      <c r="B10" s="9" t="s">
+        <v>14</v>
       </c>
       <c r="C10" s="1" t="n">
         <v>0</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E10" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="F10" s="12" t="s">
-        <v>14</v>
+      <c r="F10" s="9" t="s">
+        <v>16</v>
       </c>
       <c r="G10" s="1" t="str">
-        <f aca="false">'Room Book'!A12</f>
-        <v>T0-0-L</v>
+        <f aca="false">'Room Book'!$A$9</f>
+        <v>B0-0-L</v>
       </c>
       <c r="H10" s="3" t="str">
         <f aca="false">IF(AND(ISNUMBER(A10),ISNUMBER(C10),ISNUMBER(E10),ISTEXT(F10),ISTEXT(G10)),A10&amp;"/"&amp;C10&amp;"/"&amp;E10,"")</f>
         <v>0/0/1</v>
       </c>
       <c r="I10" s="2" t="str">
-        <f aca="false">IF(ISTEXT(G10),VLOOKUP($G10,'Room Book'!$A$7:$I$634,2,0)&amp;" "&amp;VLOOKUP($G10,'Room Book'!$A$7:$I$634,3,0)&amp;" - "&amp;VLOOKUP($G10,'Room Book'!$A$7:$I656,8,0)&amp;" - "&amp;B10&amp;" "&amp;D10,{})</f>
-        <v>Top Floor Bathroom - Ceiling light - Light &amp; Power Switch</v>
+        <f aca="false">IF(ISTEXT(G10),VLOOKUP($G10,'Room Book'!$A$7:$I$634,2,0)&amp;" "&amp;VLOOKUP($G10,'Room Book'!$A$7:$I$634,3,0)&amp;" - "&amp;VLOOKUP($G10,'Room Book'!$A$7:$I655,8,0)&amp;" - "&amp;B10&amp;" "&amp;D10,{})</f>
+        <v>Basement Office - Ceiling light - Light &amp; Power Switch</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B11" s="12" t="s">
-        <v>12</v>
+      <c r="B11" s="9" t="s">
+        <v>14</v>
       </c>
       <c r="C11" s="1" t="n">
         <v>0</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E11" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="F11" s="12" t="s">
-        <v>14</v>
+      <c r="F11" s="9" t="s">
+        <v>16</v>
       </c>
       <c r="G11" s="1" t="str">
-        <f aca="false">'Room Book'!A13</f>
-        <v>T1-0-L</v>
+        <f aca="false">'Room Book'!A12</f>
+        <v>T0-0-L</v>
       </c>
       <c r="H11" s="3" t="str">
         <f aca="false">IF(AND(ISNUMBER(A11),ISNUMBER(C11),ISNUMBER(E11),ISTEXT(F11),ISTEXT(G11)),A11&amp;"/"&amp;C11&amp;"/"&amp;E11,"")</f>
         <v>0/0/2</v>
       </c>
       <c r="I11" s="2" t="str">
-        <f aca="false">IF(ISTEXT(G11),VLOOKUP($G11,'Room Book'!$A$7:$I$634,2,0)&amp;" "&amp;VLOOKUP($G11,'Room Book'!$A$7:$I$634,3,0)&amp;" - "&amp;VLOOKUP($G11,'Room Book'!$A$7:$I657,8,0)&amp;" - "&amp;B11&amp;" "&amp;D11,{})</f>
-        <v>Top Floor Bedroom - Wall light (north) - Light &amp; Power Switch</v>
+        <f aca="false">IF(ISTEXT(G11),VLOOKUP($G11,'Room Book'!$A$7:$I$634,2,0)&amp;" "&amp;VLOOKUP($G11,'Room Book'!$A$7:$I$634,3,0)&amp;" - "&amp;VLOOKUP($G11,'Room Book'!$A$7:$I656,8,0)&amp;" - "&amp;B11&amp;" "&amp;D11,{})</f>
+        <v>Top Floor Bathroom - Ceiling light - Light &amp; Power Switch</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B12" s="12" t="s">
-        <v>12</v>
+      <c r="B12" s="9" t="s">
+        <v>14</v>
       </c>
       <c r="C12" s="1" t="n">
         <v>0</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E12" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="F12" s="12"/>
+      <c r="F12" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G12" s="1" t="str">
+        <f aca="false">'Room Book'!A13</f>
+        <v>T1-0-L</v>
+      </c>
       <c r="H12" s="3" t="str">
         <f aca="false">IF(AND(ISNUMBER(A12),ISNUMBER(C12),ISNUMBER(E12),ISTEXT(F12),ISTEXT(G12)),A12&amp;"/"&amp;C12&amp;"/"&amp;E12,"")</f>
-        <v/>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>17</v>
+        <v>0/0/3</v>
+      </c>
+      <c r="I12" s="2" t="str">
+        <f aca="false">IF(ISTEXT(G12),VLOOKUP($G12,'Room Book'!$A$7:$I$634,2,0)&amp;" "&amp;VLOOKUP($G12,'Room Book'!$A$7:$I$634,3,0)&amp;" - "&amp;VLOOKUP($G12,'Room Book'!$A$7:$I657,8,0)&amp;" - "&amp;B12&amp;" "&amp;D12,{})</f>
+        <v>Top Floor Bedroom - Wall light (north) - Light &amp; Power Switch</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B13" s="12" t="s">
-        <v>12</v>
+      <c r="B13" s="9" t="s">
+        <v>14</v>
       </c>
       <c r="C13" s="1" t="n">
         <v>0</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E13" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="F13" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="G13" s="1" t="str">
-        <f aca="false">'Room Book'!A11</f>
-        <v>B1-2-P</v>
-      </c>
+      <c r="F13" s="9"/>
       <c r="H13" s="3" t="str">
         <f aca="false">IF(AND(ISNUMBER(A13),ISNUMBER(C13),ISNUMBER(E13),ISTEXT(F13),ISTEXT(G13)),A13&amp;"/"&amp;C13&amp;"/"&amp;E13,"")</f>
-        <v>0/0/4</v>
-      </c>
-      <c r="I13" s="2" t="str">
-        <f aca="false">IF(ISTEXT(G13),VLOOKUP($G13,'Room Book'!$A$7:$I$634,2,0)&amp;" "&amp;VLOOKUP($G13,'Room Book'!$A$7:$I$634,3,0)&amp;" - "&amp;VLOOKUP($G13,'Room Book'!$A$7:$I659,8,0)&amp;" - "&amp;B13&amp;" "&amp;D13,{})</f>
-        <v>Basement Kitchen - Wall plug - next to bed. - Light &amp; Power Switch</v>
+        <v/>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B14" s="12" t="s">
-        <v>12</v>
+      <c r="B14" s="9" t="s">
+        <v>14</v>
       </c>
       <c r="C14" s="1" t="n">
         <v>0</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E14" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="F14" s="12"/>
+      <c r="F14" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G14" s="1" t="str">
+        <f aca="false">'Room Book'!A11</f>
+        <v>B1-2-P</v>
+      </c>
       <c r="H14" s="3" t="str">
         <f aca="false">IF(AND(ISNUMBER(A14),ISNUMBER(C14),ISNUMBER(E14),ISTEXT(F14),ISTEXT(G14)),A14&amp;"/"&amp;C14&amp;"/"&amp;E14,"")</f>
-        <v/>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>17</v>
+        <v>0/0/5</v>
+      </c>
+      <c r="I14" s="2" t="str">
+        <f aca="false">IF(ISTEXT(G14),VLOOKUP($G14,'Room Book'!$A$7:$I$634,2,0)&amp;" "&amp;VLOOKUP($G14,'Room Book'!$A$7:$I$634,3,0)&amp;" - "&amp;VLOOKUP($G14,'Room Book'!$A$7:$I659,8,0)&amp;" - "&amp;B14&amp;" "&amp;D14,{})</f>
+        <v>Basement Kitchen - Wall plug - next to bed. - Light &amp; Power Switch</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B15" s="12" t="s">
-        <v>12</v>
+      <c r="B15" s="9" t="s">
+        <v>14</v>
       </c>
       <c r="C15" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E15" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F15" s="12" t="str">
-        <f aca="false">F9</f>
-        <v>DPST-1-1</v>
-      </c>
-      <c r="G15" s="2" t="str">
-        <f aca="false">G9</f>
-        <v>B0-0-L</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="F15" s="9"/>
       <c r="H15" s="3" t="str">
         <f aca="false">IF(AND(ISNUMBER(A15),ISNUMBER(C15),ISNUMBER(E15),ISTEXT(F15),ISTEXT(G15)),A15&amp;"/"&amp;C15&amp;"/"&amp;E15,"")</f>
-        <v>0/1/0</v>
-      </c>
-      <c r="I15" s="2" t="str">
-        <f aca="false">IF(ISTEXT(G15),VLOOKUP($G15,'Room Book'!$A$7:$I$634,2,0)&amp;" "&amp;VLOOKUP($G15,'Room Book'!$A$7:$I$634,3,0)&amp;" - "&amp;VLOOKUP($G15,'Room Book'!$A$7:$I661,8,0)&amp;" - "&amp;B15&amp;" "&amp;D15,{})</f>
-        <v>Basement Office - Ceiling light - Light &amp; Power Status</v>
+        <v/>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B16" s="12" t="s">
-        <v>12</v>
+      <c r="B16" s="9" t="s">
+        <v>14</v>
       </c>
       <c r="C16" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E16" s="1" t="n">
+        <f aca="false">E10</f>
         <v>1</v>
       </c>
-      <c r="F16" s="12" t="str">
+      <c r="F16" s="9" t="str">
         <f aca="false">F10</f>
         <v>DPST-1-1</v>
       </c>
       <c r="G16" s="2" t="str">
         <f aca="false">G10</f>
-        <v>T0-0-L</v>
+        <v>B0-0-L</v>
       </c>
       <c r="H16" s="3" t="str">
         <f aca="false">IF(AND(ISNUMBER(A16),ISNUMBER(C16),ISNUMBER(E16),ISTEXT(F16),ISTEXT(G16)),A16&amp;"/"&amp;C16&amp;"/"&amp;E16,"")</f>
         <v>0/1/1</v>
       </c>
       <c r="I16" s="2" t="str">
-        <f aca="false">IF(ISTEXT(G16),VLOOKUP($G16,'Room Book'!$A$7:$I$634,2,0)&amp;" "&amp;VLOOKUP($G16,'Room Book'!$A$7:$I$634,3,0)&amp;" - "&amp;VLOOKUP($G16,'Room Book'!$A$7:$I662,8,0)&amp;" - "&amp;B16&amp;" "&amp;D16,{})</f>
-        <v>Top Floor Bathroom - Ceiling light - Light &amp; Power Status</v>
+        <f aca="false">IF(ISTEXT(G16),VLOOKUP($G16,'Room Book'!$A$7:$I$634,2,0)&amp;" "&amp;VLOOKUP($G16,'Room Book'!$A$7:$I$634,3,0)&amp;" - "&amp;VLOOKUP($G16,'Room Book'!$A$7:$I661,8,0)&amp;" - "&amp;B16&amp;" "&amp;D16,{})</f>
+        <v>Basement Office - Ceiling light - Light &amp; Power Status</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B17" s="12" t="s">
-        <v>12</v>
+      <c r="B17" s="9" t="s">
+        <v>14</v>
       </c>
       <c r="C17" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E17" s="1" t="n">
+        <f aca="false">E11</f>
         <v>2</v>
       </c>
-      <c r="F17" s="12" t="str">
+      <c r="F17" s="9" t="str">
         <f aca="false">F11</f>
         <v>DPST-1-1</v>
       </c>
       <c r="G17" s="2" t="str">
         <f aca="false">G11</f>
-        <v>T1-0-L</v>
+        <v>T0-0-L</v>
       </c>
       <c r="H17" s="3" t="str">
         <f aca="false">IF(AND(ISNUMBER(A17),ISNUMBER(C17),ISNUMBER(E17),ISTEXT(F17),ISTEXT(G17)),A17&amp;"/"&amp;C17&amp;"/"&amp;E17,"")</f>
         <v>0/1/2</v>
       </c>
       <c r="I17" s="2" t="str">
-        <f aca="false">IF(ISTEXT(G17),VLOOKUP($G17,'Room Book'!$A$7:$I$634,2,0)&amp;" "&amp;VLOOKUP($G17,'Room Book'!$A$7:$I$634,3,0)&amp;" - "&amp;VLOOKUP($G17,'Room Book'!$A$7:$I663,8,0)&amp;" - "&amp;B17&amp;" "&amp;D17,{})</f>
-        <v>Top Floor Bedroom - Wall light (north) - Light &amp; Power Status</v>
+        <f aca="false">IF(ISTEXT(G17),VLOOKUP($G17,'Room Book'!$A$7:$I$634,2,0)&amp;" "&amp;VLOOKUP($G17,'Room Book'!$A$7:$I$634,3,0)&amp;" - "&amp;VLOOKUP($G17,'Room Book'!$A$7:$I662,8,0)&amp;" - "&amp;B17&amp;" "&amp;D17,{})</f>
+        <v>Top Floor Bathroom - Ceiling light - Light &amp; Power Status</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B18" s="12" t="s">
-        <v>12</v>
+      <c r="B18" s="9" t="s">
+        <v>14</v>
       </c>
       <c r="C18" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E18" s="1" t="n">
+        <f aca="false">E12</f>
         <v>3</v>
       </c>
-      <c r="F18" s="12"/>
-      <c r="G18" s="2"/>
+      <c r="F18" s="9" t="str">
+        <f aca="false">F12</f>
+        <v>DPST-1-1</v>
+      </c>
+      <c r="G18" s="2" t="str">
+        <f aca="false">G12</f>
+        <v>T1-0-L</v>
+      </c>
       <c r="H18" s="3" t="str">
         <f aca="false">IF(AND(ISNUMBER(A18),ISNUMBER(C18),ISNUMBER(E18),ISTEXT(F18),ISTEXT(G18)),A18&amp;"/"&amp;C18&amp;"/"&amp;E18,"")</f>
-        <v/>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>17</v>
+        <v>0/1/3</v>
+      </c>
+      <c r="I18" s="2" t="str">
+        <f aca="false">IF(ISTEXT(G18),VLOOKUP($G18,'Room Book'!$A$7:$I$634,2,0)&amp;" "&amp;VLOOKUP($G18,'Room Book'!$A$7:$I$634,3,0)&amp;" - "&amp;VLOOKUP($G18,'Room Book'!$A$7:$I663,8,0)&amp;" - "&amp;B18&amp;" "&amp;D18,{})</f>
+        <v>Top Floor Bedroom - Wall light (north) - Light &amp; Power Status</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B19" s="12" t="s">
-        <v>12</v>
+      <c r="B19" s="9" t="s">
+        <v>14</v>
       </c>
       <c r="C19" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E19" s="1" t="n">
+        <f aca="false">E13</f>
         <v>4</v>
       </c>
-      <c r="F19" s="12" t="str">
-        <f aca="false">F13</f>
-        <v>DPST-1-1</v>
-      </c>
-      <c r="G19" s="2" t="str">
-        <f aca="false">G13</f>
-        <v>B1-2-P</v>
-      </c>
+      <c r="F19" s="9"/>
+      <c r="G19" s="2"/>
       <c r="H19" s="3" t="str">
         <f aca="false">IF(AND(ISNUMBER(A19),ISNUMBER(C19),ISNUMBER(E19),ISTEXT(F19),ISTEXT(G19)),A19&amp;"/"&amp;C19&amp;"/"&amp;E19,"")</f>
-        <v>0/1/4</v>
-      </c>
-      <c r="I19" s="2" t="str">
-        <f aca="false">IF(ISTEXT(G19),VLOOKUP($G19,'Room Book'!$A$7:$I$634,2,0)&amp;" "&amp;VLOOKUP($G19,'Room Book'!$A$7:$I$634,3,0)&amp;" - "&amp;VLOOKUP($G19,'Room Book'!$A$7:$I665,8,0)&amp;" - "&amp;B19&amp;" "&amp;D19,{})</f>
-        <v>Basement Kitchen - Wall plug - next to bed. - Light &amp; Power Status</v>
+        <v/>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B20" s="12" t="s">
-        <v>12</v>
+      <c r="B20" s="9" t="s">
+        <v>14</v>
       </c>
       <c r="C20" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E20" s="1" t="n">
+        <f aca="false">E14</f>
         <v>5</v>
       </c>
-      <c r="F20" s="12"/>
+      <c r="F20" s="9" t="str">
+        <f aca="false">F14</f>
+        <v>DPST-1-1</v>
+      </c>
+      <c r="G20" s="2" t="str">
+        <f aca="false">G14</f>
+        <v>B1-2-P</v>
+      </c>
       <c r="H20" s="3" t="str">
         <f aca="false">IF(AND(ISNUMBER(A20),ISNUMBER(C20),ISNUMBER(E20),ISTEXT(F20),ISTEXT(G20)),A20&amp;"/"&amp;C20&amp;"/"&amp;E20,"")</f>
-        <v/>
-      </c>
-      <c r="J20" s="2" t="s">
-        <v>17</v>
+        <v>0/1/5</v>
+      </c>
+      <c r="I20" s="2" t="str">
+        <f aca="false">IF(ISTEXT(G20),VLOOKUP($G20,'Room Book'!$A$7:$I$634,2,0)&amp;" "&amp;VLOOKUP($G20,'Room Book'!$A$7:$I$634,3,0)&amp;" - "&amp;VLOOKUP($G20,'Room Book'!$A$7:$I665,8,0)&amp;" - "&amp;B20&amp;" "&amp;D20,{})</f>
+        <v>Basement Kitchen - Wall plug - next to bed. - Light &amp; Power Status</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="9"/>
-      <c r="B21" s="10"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="10"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="9"/>
-      <c r="I21" s="9"/>
-      <c r="J21" s="9"/>
+      <c r="A21" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E21" s="1" t="n">
+        <f aca="false">E15</f>
+        <v>6</v>
+      </c>
+      <c r="F21" s="9"/>
+      <c r="H21" s="3" t="str">
+        <f aca="false">IF(AND(ISNUMBER(A21),ISNUMBER(C21),ISNUMBER(E21),ISTEXT(F21),ISTEXT(G21)),A21&amp;"/"&amp;C21&amp;"/"&amp;E21,"")</f>
+        <v/>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="B22" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="C22" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="D22" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="E22" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G22" s="13" t="str">
-        <f aca="false">'Room Book'!A10</f>
-        <v>B0-1-B</v>
-      </c>
-      <c r="H22" s="3" t="str">
-        <f aca="false">IF(AND(ISNUMBER(A22),ISNUMBER(C22),ISNUMBER(E22),ISTEXT(F22),ISTEXT(G22)),A22&amp;"/"&amp;C22&amp;"/"&amp;E22,"")</f>
-        <v>1/0/0</v>
-      </c>
-      <c r="I22" s="2" t="str">
-        <f aca="false">IF(ISTEXT(G22),VLOOKUP($G22,'Room Book'!$A$7:$I$634,2,0)&amp;" "&amp;VLOOKUP($G22,'Room Book'!$A$7:$I$634,3,0)&amp;" - "&amp;VLOOKUP($G22,'Room Book'!$A$7:$I668,8,0)&amp;" - "&amp;B22&amp;" "&amp;D22,{})</f>
-        <v>Basement Office - Blinds - Blinds Up/Down</v>
-      </c>
-      <c r="J22" s="15"/>
+      <c r="A22" s="10"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="10"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="13" t="n">
         <v>1</v>
       </c>
       <c r="B23" s="14" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C23" s="13" t="n">
         <v>0</v>
       </c>
       <c r="D23" s="15" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E23" s="13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G23" s="13" t="str">
-        <f aca="false">'Room Book'!A14</f>
-        <v>T1-1-B</v>
+        <f aca="false">'Room Book'!A10</f>
+        <v>B0-1-B</v>
       </c>
       <c r="H23" s="3" t="str">
         <f aca="false">IF(AND(ISNUMBER(A23),ISNUMBER(C23),ISNUMBER(E23),ISTEXT(F23),ISTEXT(G23)),A23&amp;"/"&amp;C23&amp;"/"&amp;E23,"")</f>
-        <v>1/0/1</v>
+        <v>1/0/0</v>
       </c>
       <c r="I23" s="2" t="str">
-        <f aca="false">IF(ISTEXT(G23),VLOOKUP($G23,'Room Book'!$A$7:$I$634,2,0)&amp;" "&amp;VLOOKUP($G23,'Room Book'!$A$7:$I$634,3,0)&amp;" - "&amp;VLOOKUP($G23,'Room Book'!$A$7:$I669,8,0)&amp;" - "&amp;B23&amp;" "&amp;D23,{})</f>
-        <v>Top Floor Bedroom - Blinds (east) - Blinds Up/Down</v>
-      </c>
+        <f aca="false">IF(ISTEXT(G23),VLOOKUP($G23,'Room Book'!$A$7:$I$634,2,0)&amp;" "&amp;VLOOKUP($G23,'Room Book'!$A$7:$I$634,3,0)&amp;" - "&amp;VLOOKUP($G23,'Room Book'!$A$7:$I668,8,0)&amp;" - "&amp;B23&amp;" "&amp;D23,{})</f>
+        <v>Basement Office - Blinds - Blinds Up/Down</v>
+      </c>
+      <c r="J23" s="15"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="13" t="n">
         <v>1</v>
       </c>
       <c r="B24" s="14" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C24" s="13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D24" s="15" t="s">
         <v>22</v>
       </c>
       <c r="E24" s="13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="G24" s="13" t="str">
-        <f aca="false">G22</f>
-        <v>B0-1-B</v>
+        <f aca="false">'Room Book'!A14</f>
+        <v>T1-1-B</v>
       </c>
       <c r="H24" s="3" t="str">
         <f aca="false">IF(AND(ISNUMBER(A24),ISNUMBER(C24),ISNUMBER(E24),ISTEXT(F24),ISTEXT(G24)),A24&amp;"/"&amp;C24&amp;"/"&amp;E24,"")</f>
-        <v>1/1/0</v>
+        <v>1/0/1</v>
       </c>
       <c r="I24" s="2" t="str">
-        <f aca="false">IF(ISTEXT(G24),VLOOKUP($G24,'Room Book'!$A$7:$I$634,2,0)&amp;" "&amp;VLOOKUP($G24,'Room Book'!$A$7:$I$634,3,0)&amp;" - "&amp;VLOOKUP($G24,'Room Book'!$A$7:$I670,8,0)&amp;" - "&amp;B24&amp;" "&amp;D24,{})</f>
-        <v>Basement Office - Blinds - Blinds Stop</v>
-      </c>
-      <c r="J24" s="15"/>
+        <f aca="false">IF(ISTEXT(G24),VLOOKUP($G24,'Room Book'!$A$7:$I$634,2,0)&amp;" "&amp;VLOOKUP($G24,'Room Book'!$A$7:$I$634,3,0)&amp;" - "&amp;VLOOKUP($G24,'Room Book'!$A$7:$I669,8,0)&amp;" - "&amp;B24&amp;" "&amp;D24,{})</f>
+        <v>Top Floor Bedroom - Blinds (east) - Blinds Up/Down</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="13" t="n">
         <v>1</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C25" s="13" t="n">
         <v>1</v>
       </c>
       <c r="D25" s="15" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E25" s="13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G25" s="13" t="str">
         <f aca="false">G23</f>
-        <v>T1-1-B</v>
+        <v>B0-1-B</v>
       </c>
       <c r="H25" s="3" t="str">
         <f aca="false">IF(AND(ISNUMBER(A25),ISNUMBER(C25),ISNUMBER(E25),ISTEXT(F25),ISTEXT(G25)),A25&amp;"/"&amp;C25&amp;"/"&amp;E25,"")</f>
-        <v>1/1/1</v>
+        <v>1/1/0</v>
       </c>
       <c r="I25" s="2" t="str">
-        <f aca="false">IF(ISTEXT(G25),VLOOKUP($G25,'Room Book'!$A$7:$I$634,2,0)&amp;" "&amp;VLOOKUP($G25,'Room Book'!$A$7:$I$634,3,0)&amp;" - "&amp;VLOOKUP($G25,'Room Book'!$A$7:$I671,8,0)&amp;" - "&amp;B25&amp;" "&amp;D25,{})</f>
-        <v>Top Floor Bedroom - Blinds (east) - Blinds Stop</v>
-      </c>
+        <f aca="false">IF(ISTEXT(G25),VLOOKUP($G25,'Room Book'!$A$7:$I$634,2,0)&amp;" "&amp;VLOOKUP($G25,'Room Book'!$A$7:$I$634,3,0)&amp;" - "&amp;VLOOKUP($G25,'Room Book'!$A$7:$I670,8,0)&amp;" - "&amp;B25&amp;" "&amp;D25,{})</f>
+        <v>Basement Office - Blinds - Blinds Stop</v>
+      </c>
+      <c r="J25" s="15"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="13" t="n">
         <v>1</v>
       </c>
       <c r="B26" s="14" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C26" s="13" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D26" s="15" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E26" s="13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G26" s="14" t="str">
-        <f aca="false">G22</f>
-        <v>B0-1-B</v>
+        <v>16</v>
+      </c>
+      <c r="G26" s="13" t="str">
+        <f aca="false">G24</f>
+        <v>T1-1-B</v>
       </c>
       <c r="H26" s="3" t="str">
         <f aca="false">IF(AND(ISNUMBER(A26),ISNUMBER(C26),ISNUMBER(E26),ISTEXT(F26),ISTEXT(G26)),A26&amp;"/"&amp;C26&amp;"/"&amp;E26,"")</f>
-        <v>1/2/0</v>
+        <v>1/1/1</v>
       </c>
       <c r="I26" s="2" t="str">
-        <f aca="false">IF(ISTEXT(G26),VLOOKUP($G26,'Room Book'!$A$7:$I$634,2,0)&amp;" "&amp;VLOOKUP($G26,'Room Book'!$A$7:$I$634,3,0)&amp;" - "&amp;VLOOKUP($G26,'Room Book'!$A$7:$I672,8,0)&amp;" - "&amp;B26&amp;" "&amp;D26,{})</f>
-        <v>Basement Office - Blinds - Blinds Absolute Position</v>
-      </c>
-      <c r="J26" s="15"/>
+        <f aca="false">IF(ISTEXT(G26),VLOOKUP($G26,'Room Book'!$A$7:$I$634,2,0)&amp;" "&amp;VLOOKUP($G26,'Room Book'!$A$7:$I$634,3,0)&amp;" - "&amp;VLOOKUP($G26,'Room Book'!$A$7:$I671,8,0)&amp;" - "&amp;B26&amp;" "&amp;D26,{})</f>
+        <v>Top Floor Bedroom - Blinds (east) - Blinds Stop</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="13" t="n">
         <v>1</v>
       </c>
       <c r="B27" s="14" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C27" s="13" t="n">
         <v>2</v>
       </c>
       <c r="D27" s="15" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E27" s="13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G27" s="14" t="str">
         <f aca="false">G23</f>
-        <v>T1-1-B</v>
+        <v>B0-1-B</v>
       </c>
       <c r="H27" s="3" t="str">
         <f aca="false">IF(AND(ISNUMBER(A27),ISNUMBER(C27),ISNUMBER(E27),ISTEXT(F27),ISTEXT(G27)),A27&amp;"/"&amp;C27&amp;"/"&amp;E27,"")</f>
-        <v>1/2/1</v>
+        <v>1/2/0</v>
       </c>
       <c r="I27" s="2" t="str">
-        <f aca="false">IF(ISTEXT(G27),VLOOKUP($G27,'Room Book'!$A$7:$I$634,2,0)&amp;" "&amp;VLOOKUP($G27,'Room Book'!$A$7:$I$634,3,0)&amp;" - "&amp;VLOOKUP($G27,'Room Book'!$A$7:$I673,8,0)&amp;" - "&amp;B27&amp;" "&amp;D27,{})</f>
-        <v>Top Floor Bedroom - Blinds (east) - Blinds Absolute Position</v>
-      </c>
+        <f aca="false">IF(ISTEXT(G27),VLOOKUP($G27,'Room Book'!$A$7:$I$634,2,0)&amp;" "&amp;VLOOKUP($G27,'Room Book'!$A$7:$I$634,3,0)&amp;" - "&amp;VLOOKUP($G27,'Room Book'!$A$7:$I672,8,0)&amp;" - "&amp;B27&amp;" "&amp;D27,{})</f>
+        <v>Basement Office - Blinds - Blinds Absolute Position</v>
+      </c>
+      <c r="J27" s="15"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="13" t="n">
         <v>1</v>
       </c>
       <c r="B28" s="14" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C28" s="13" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D28" s="15" t="s">
         <v>25</v>
       </c>
       <c r="E28" s="13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G28" s="13" t="str">
-        <f aca="false">G22</f>
-        <v>B0-1-B</v>
+        <v>26</v>
+      </c>
+      <c r="G28" s="14" t="str">
+        <f aca="false">G24</f>
+        <v>T1-1-B</v>
       </c>
       <c r="H28" s="3" t="str">
         <f aca="false">IF(AND(ISNUMBER(A28),ISNUMBER(C28),ISNUMBER(E28),ISTEXT(F28),ISTEXT(G28)),A28&amp;"/"&amp;C28&amp;"/"&amp;E28,"")</f>
-        <v>1/4/0</v>
+        <v>1/2/1</v>
       </c>
       <c r="I28" s="2" t="str">
-        <f aca="false">IF(ISTEXT(G28),VLOOKUP($G28,'Room Book'!$A$7:$I$634,2,0)&amp;" "&amp;VLOOKUP($G28,'Room Book'!$A$7:$I$634,3,0)&amp;" - "&amp;VLOOKUP($G28,'Room Book'!$A$7:$I674,8,0)&amp;" - "&amp;B28&amp;" "&amp;D28,{})</f>
-        <v>Basement Office - Blinds - Blinds Status Position</v>
-      </c>
-      <c r="J28" s="15"/>
+        <f aca="false">IF(ISTEXT(G28),VLOOKUP($G28,'Room Book'!$A$7:$I$634,2,0)&amp;" "&amp;VLOOKUP($G28,'Room Book'!$A$7:$I$634,3,0)&amp;" - "&amp;VLOOKUP($G28,'Room Book'!$A$7:$I673,8,0)&amp;" - "&amp;B28&amp;" "&amp;D28,{})</f>
+        <v>Top Floor Bedroom - Blinds (east) - Blinds Absolute Position</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="13" t="n">
         <v>1</v>
       </c>
       <c r="B29" s="14" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C29" s="13" t="n">
         <v>4</v>
       </c>
       <c r="D29" s="15" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E29" s="13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G29" s="13" t="str">
         <f aca="false">G23</f>
-        <v>T1-1-B</v>
+        <v>B0-1-B</v>
       </c>
       <c r="H29" s="3" t="str">
         <f aca="false">IF(AND(ISNUMBER(A29),ISNUMBER(C29),ISNUMBER(E29),ISTEXT(F29),ISTEXT(G29)),A29&amp;"/"&amp;C29&amp;"/"&amp;E29,"")</f>
+        <v>1/4/0</v>
+      </c>
+      <c r="I29" s="2" t="str">
+        <f aca="false">IF(ISTEXT(G29),VLOOKUP($G29,'Room Book'!$A$7:$I$634,2,0)&amp;" "&amp;VLOOKUP($G29,'Room Book'!$A$7:$I$634,3,0)&amp;" - "&amp;VLOOKUP($G29,'Room Book'!$A$7:$I674,8,0)&amp;" - "&amp;B29&amp;" "&amp;D29,{})</f>
+        <v>Basement Office - Blinds - Blinds Status Position</v>
+      </c>
+      <c r="J29" s="15"/>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="B30" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C30" s="13" t="n">
+        <v>4</v>
+      </c>
+      <c r="D30" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E30" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G30" s="13" t="str">
+        <f aca="false">G24</f>
+        <v>T1-1-B</v>
+      </c>
+      <c r="H30" s="3" t="str">
+        <f aca="false">IF(AND(ISNUMBER(A30),ISNUMBER(C30),ISNUMBER(E30),ISTEXT(F30),ISTEXT(G30)),A30&amp;"/"&amp;C30&amp;"/"&amp;E30,"")</f>
         <v>1/4/1</v>
       </c>
-      <c r="I29" s="2" t="str">
-        <f aca="false">IF(ISTEXT(G29),VLOOKUP($G29,'Room Book'!$A$7:$I$634,2,0)&amp;" "&amp;VLOOKUP($G29,'Room Book'!$A$7:$I$634,3,0)&amp;" - "&amp;VLOOKUP($G29,'Room Book'!$A$7:$I675,8,0)&amp;" - "&amp;B29&amp;" "&amp;D29,{})</f>
+      <c r="I30" s="2" t="str">
+        <f aca="false">IF(ISTEXT(G30),VLOOKUP($G30,'Room Book'!$A$7:$I$634,2,0)&amp;" "&amp;VLOOKUP($G30,'Room Book'!$A$7:$I$634,3,0)&amp;" - "&amp;VLOOKUP($G30,'Room Book'!$A$7:$I675,8,0)&amp;" - "&amp;B30&amp;" "&amp;D30,{})</f>
         <v>Top Floor Bedroom - Blinds (east) - Blinds Status Position</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H30" s="3" t="str">
-        <f aca="false">IF(AND(ISNUMBER(A30),ISNUMBER(C30),ISNUMBER(E30)),A30&amp;"/"&amp;C30&amp;"/"&amp;E30,"")</f>
-        <v/>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3240,8 +3263,14 @@
         <v/>
       </c>
     </row>
+    <row r="278" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H278" s="3" t="str">
+        <f aca="false">IF(AND(ISNUMBER(A278),ISNUMBER(C278),ISNUMBER(E278)),A278&amp;"/"&amp;C278&amp;"/"&amp;E278,"")</f>
+        <v/>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A7:J277"/>
+  <autoFilter ref="A7:J278"/>
   <mergeCells count="3">
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A4:B4"/>
@@ -3266,7 +3295,7 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I9" activeCellId="1" sqref="J20 I9"/>
+      <selection pane="topLeft" activeCell="I9" activeCellId="0" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3285,7 +3314,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="17" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3293,31 +3322,31 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3326,28 +3355,28 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="I8" s="18" t="s">
         <v>11</v>
@@ -3359,25 +3388,25 @@
         <v>B0-0-L</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E9" s="1" t="n">
         <v>0</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="I9" s="2"/>
     </row>
@@ -3387,25 +3416,25 @@
         <v>B0-1-B</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E10" s="1" t="n">
         <v>1</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="I10" s="2"/>
     </row>
@@ -3415,25 +3444,25 @@
         <v>B1-2-P</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E11" s="1" t="n">
         <v>2</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I11" s="2"/>
     </row>
@@ -3443,25 +3472,25 @@
         <v>T0-0-L</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E12" s="1" t="n">
         <v>0</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3470,25 +3499,25 @@
         <v>T1-0-L</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E13" s="1" t="n">
         <v>0</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3497,25 +3526,25 @@
         <v>T1-1-B</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E14" s="1" t="n">
         <v>1</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>